<commit_message>
Add project for week8 experiment (ElapsedTime)
</commit_message>
<xml_diff>
--- a/Actividad_FormatoInstruciones16BitsSem6Arq (202020).xlsx
+++ b/Actividad_FormatoInstruciones16BitsSem6Arq (202020).xlsx
@@ -4235,8 +4235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>